<commit_message>
Code formatting changes. A couple more OCXOs.
</commit_message>
<xml_diff>
--- a/AlternateXOs.xlsx
+++ b/AlternateXOs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
   <si>
     <t>MFR</t>
   </si>
@@ -167,6 +167,27 @@
   </si>
   <si>
     <t>12x18</t>
+  </si>
+  <si>
+    <t>Abracon Corp</t>
+  </si>
+  <si>
+    <t>0-50</t>
+  </si>
+  <si>
+    <t>5/3.3</t>
+  </si>
+  <si>
+    <t>25.4x22.1</t>
+  </si>
+  <si>
+    <t>AOCJY-16.384MHZ</t>
+  </si>
+  <si>
+    <t>OX914xS3</t>
+  </si>
+  <si>
+    <t>-55-85</t>
   </si>
 </sst>
 </file>
@@ -574,7 +595,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,38 +1014,101 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="2"/>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>20</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="3">
+        <v>10</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="6">
+        <v>160.80000000000001</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" s="8">
+        <f>N13/3.3*1000</f>
+        <v>1090.909090909091</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>140</v>
+      </c>
+      <c r="F14" s="3">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3">
+        <v>40</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I14" s="3">
+        <v>20</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="6">
+        <v>42</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3.3</v>
+      </c>
       <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="2"/>
+      <c r="N14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
Investigated a couple more XOs
</commit_message>
<xml_diff>
--- a/AlternateXOs.xlsx
+++ b/AlternateXOs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>MFR</t>
   </si>
@@ -188,6 +188,27 @@
   </si>
   <si>
     <t>-55-85</t>
+  </si>
+  <si>
+    <t>FOX</t>
+  </si>
+  <si>
+    <t>FOX924B</t>
+  </si>
+  <si>
+    <t>HCMOS</t>
+  </si>
+  <si>
+    <t>-30-85</t>
+  </si>
+  <si>
+    <t>TXC Corp</t>
+  </si>
+  <si>
+    <t>7N-20.000MBP-T</t>
+  </si>
+  <si>
+    <t>1ppm/yr</t>
   </si>
 </sst>
 </file>
@@ -592,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,13 +724,11 @@
       <c r="F3" s="10">
         <v>300</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10">
-        <v>1</v>
-      </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
+      <c r="G3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="12" t="s">
         <v>42</v>
       </c>
@@ -1326,21 +1345,96 @@
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F20" s="3">
+        <v>300</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="6">
+        <v>6.41</v>
+      </c>
+      <c r="L20" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>6</v>
+      </c>
       <c r="N20" s="3"/>
-      <c r="O20" s="2"/>
+      <c r="O20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>280</v>
+      </c>
+      <c r="F21" s="3">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I21" s="3">
+        <v>20</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="6">
+        <v>10.89</v>
+      </c>
+      <c r="L21" s="3">
+        <v>5</v>
+      </c>
+      <c r="M21" s="3">
+        <v>10</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:K9">

</xml_diff>